<commit_message>
bug fix for reset command
</commit_message>
<xml_diff>
--- a/gameData/shared/Houses.xlsx
+++ b/gameData/shared/Houses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="480" windowWidth="16420" windowHeight="9280" tabRatio="883"/>
+    <workbookView xWindow="10220" yWindow="1840" windowWidth="16420" windowHeight="10080" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="houses" sheetId="2" r:id="rId1"/>
@@ -753,7 +753,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -780,10 +780,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -794,10 +794,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -808,10 +808,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -822,10 +822,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -836,10 +836,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
modify configs and and create house count limit
</commit_message>
<xml_diff>
--- a/gameData/shared/Houses.xlsx
+++ b/gameData/shared/Houses.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="5420" yWindow="3340" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="houses" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>INT_height</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -56,22 +56,6 @@
   </si>
   <si>
     <t>dwelling</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>woodcutter</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>farmer</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>quarrier</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>miner</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -105,6 +89,45 @@
   <si>
     <t>STR_type</t>
     <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_limitBy</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>townHall</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>lumbermill</t>
+  </si>
+  <si>
+    <t>mill</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>stoneMason</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>foundry</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>woodcutter</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>farmer</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>quarrier</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>miner</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -253,7 +276,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -286,6 +309,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -299,7 +326,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="28">
+  <cellStyles count="32">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -316,6 +343,8 @@
     <cellStyle name="超链接" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -325,6 +354,8 @@
     <cellStyle name="访问过的超链接" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -774,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -785,9 +816,9 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -796,13 +827,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+    <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -813,77 +847,92 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="20" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
+    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="20" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="20" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="20" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>